<commit_message>
Cleaned up spreadsheet with clubs in Brabant Oost.
</commit_message>
<xml_diff>
--- a/Photo Club Hub/ViewModel/Lists/241113_Fotoclubs_Brabant_Oost.xlsx
+++ b/Photo Club Hub/ViewModel/Lists/241113_Fotoclubs_Brabant_Oost.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/ViewModel/Lists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370D6A7D-02EF-F940-986A-A6167E609BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E5B4E3-900C-B54B-AC8D-09B663F433A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25680" yWindow="660" windowWidth="25360" windowHeight="26260" xr2:uid="{9FE4029D-0EDD-9D45-9625-9F901A7640D3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="148">
   <si>
     <t>Fotoclub</t>
   </si>
@@ -438,9 +438,6 @@
   </si>
   <si>
     <t>Lievendaal (bestaat dit nog?)</t>
-  </si>
-  <si>
-    <t>Nee</t>
   </si>
   <si>
     <t>Luminos</t>
@@ -578,7 +575,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7D8B52F3-C586-3040-894D-6E64EBE279E8}" name="Table1" displayName="Table1" ref="A1:F65" totalsRowShown="0">
-  <autoFilter ref="A1:F65" xr:uid="{7D8B52F3-C586-3040-894D-6E64EBE279E8}"/>
+  <autoFilter ref="A1:F65" xr:uid="{7D8B52F3-C586-3040-894D-6E64EBE279E8}">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="-"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F65">
     <sortCondition ref="D1:D65"/>
   </sortState>
@@ -895,7 +898,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C64" sqref="C64"/>
+      <selection pane="bottomLeft" activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -921,13 +924,13 @@
         <v>76</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -945,7 +948,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -958,11 +961,11 @@
       <c r="D3" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>1608</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>80</v>
       </c>
@@ -1000,13 +1003,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>139</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>81</v>
@@ -1023,7 +1026,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="5" t="s">
@@ -1034,7 +1037,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>25</v>
       </c>
@@ -1068,7 +1071,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>0</v>
       </c>
@@ -1086,7 +1089,7 @@
         <v>1611</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>25</v>
       </c>
@@ -1104,7 +1107,7 @@
         <v>1681</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>39</v>
       </c>
@@ -1140,7 +1143,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>0</v>
       </c>
@@ -1176,7 +1179,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>0</v>
       </c>
@@ -1194,7 +1197,7 @@
         <v>1616</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>0</v>
       </c>
@@ -1244,7 +1247,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>0</v>
       </c>
@@ -1262,7 +1265,7 @@
         <v>1620</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>0</v>
       </c>
@@ -1300,7 +1303,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>0</v>
       </c>
@@ -1336,7 +1339,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>0</v>
       </c>
@@ -1354,7 +1357,7 @@
         <v>1643</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>0</v>
       </c>
@@ -1380,19 +1383,17 @@
         <v>133</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="E27" s="5" t="s">
-        <v>134</v>
-      </c>
+      <c r="E27" s="5"/>
       <c r="F27" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>0</v>
       </c>
@@ -1415,11 +1416,11 @@
         <v>0</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>130</v>
@@ -1433,11 +1434,11 @@
         <v>25</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>130</v>
@@ -1446,7 +1447,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>0</v>
       </c>
@@ -1464,7 +1465,7 @@
         <v>1632</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>0</v>
       </c>
@@ -1547,7 +1548,7 @@
         <v>69</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>130</v>
@@ -1597,7 +1598,7 @@
         <v>0</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C39" s="6"/>
       <c r="D39" s="5" t="s">
@@ -1630,7 +1631,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
         <v>0</v>
       </c>
@@ -1648,7 +1649,7 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
         <v>25</v>
       </c>
@@ -1686,7 +1687,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
         <v>4</v>
       </c>
@@ -1718,7 +1719,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
         <v>0</v>
       </c>
@@ -1734,7 +1735,7 @@
         <v>1683</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
         <v>0</v>
       </c>
@@ -1750,7 +1751,7 @@
         <v>1631</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
         <v>30</v>
       </c>
@@ -1768,7 +1769,7 @@
         <v>1676</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
         <v>4</v>
       </c>
@@ -1779,11 +1780,11 @@
       <c r="D49" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="E49">
+      <c r="F49">
         <v>1615</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
         <v>0</v>
       </c>
@@ -1794,7 +1795,7 @@
       <c r="D50" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="E50">
+      <c r="F50">
         <v>1668</v>
       </c>
     </row>
@@ -1834,7 +1835,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
         <v>0</v>
       </c>
@@ -1844,11 +1845,11 @@
       <c r="D53" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="E53">
+      <c r="F53">
         <v>1619</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
         <v>0</v>
       </c>
@@ -1880,7 +1881,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
         <v>25</v>
       </c>
@@ -1896,7 +1897,7 @@
         <v>1637</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
         <v>0</v>
       </c>
@@ -1916,10 +1917,10 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>54</v>
@@ -1934,7 +1935,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
         <v>25</v>
       </c>
@@ -1950,7 +1951,7 @@
         <v>1661</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
         <v>25</v>
       </c>
@@ -1966,7 +1967,7 @@
         <v>1634</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
         <v>120</v>
       </c>
@@ -1982,7 +1983,7 @@
         <v>1678</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
         <v>0</v>
       </c>
@@ -2013,11 +2014,12 @@
       <c r="D63" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="E63" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E63"/>
+      <c r="F63" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
         <v>0</v>
       </c>
@@ -2053,7 +2055,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E67" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F67" s="4">
         <f>COUNTA(B2:B205)</f>

</xml_diff>